<commit_message>
Added power value and power value upgrades to the mix which works.
Next steps:
Multi unlocks/multi upgrades for production and demand
Prestige System
Tracking more stats and defining what needs to be plotted and how to optimize.
</commit_message>
<xml_diff>
--- a/IdlePowerBalancing.xlsx
+++ b/IdlePowerBalancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\PycharmProjects\IdlePowerBalancing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01959AC9-A81A-4512-846A-EA7C9ED55DF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B239E6-F067-4DD8-8C1F-6C786995F308}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-4147" windowWidth="28995" windowHeight="15795" tabRatio="743" activeTab="2" xr2:uid="{28C085D8-E2A0-418F-8928-7A7EE2BAEA8D}"/>
+    <workbookView xWindow="14303" yWindow="-4147" windowWidth="28995" windowHeight="15795" tabRatio="743" firstSheet="3" activeTab="7" xr2:uid="{28C085D8-E2A0-418F-8928-7A7EE2BAEA8D}"/>
   </bookViews>
   <sheets>
     <sheet name="prod_base_values" sheetId="1" r:id="rId1"/>
@@ -1327,7 +1327,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4855,7 +4855,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D25"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5252,8 +5252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFB339A-9F26-40E8-8660-93FF6C44D829}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7411,7 +7411,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8267,7 +8267,7 @@
   <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9436,14 +9436,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E531F0-085D-46CD-AA09-287683333E46}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="14"/>
-    <col min="4" max="4" width="7.7109375" style="14" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" style="14"/>
+    <col min="3" max="3" width="14.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="14" customWidth="1"/>
     <col min="5" max="6" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
@@ -9497,7 +9498,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5" s="18">
         <v>0.1</v>

</xml_diff>

<commit_message>
Added multi unlock and first parts of prestige system. Now working on profiling the code to optimize speed a little bit better. Then the next steps will be to add in the rest of the prestige functionality.
Speed optimization looks like it will rely in improving the calculation of the scores currently, which might in turn rely on optimizing the calculation speed of the resource costs (exponents of 100's or 1000's are relatively common in current implementation)
</commit_message>
<xml_diff>
--- a/IdlePowerBalancing.xlsx
+++ b/IdlePowerBalancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\PycharmProjects\IdlePowerBalancing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B239E6-F067-4DD8-8C1F-6C786995F308}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9C1C90-F678-40C4-9AE2-C7692C70DF3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-4147" windowWidth="28995" windowHeight="15795" tabRatio="743" firstSheet="3" activeTab="7" xr2:uid="{28C085D8-E2A0-418F-8928-7A7EE2BAEA8D}"/>
+    <workbookView xWindow="14303" yWindow="-4147" windowWidth="28995" windowHeight="15795" tabRatio="743" firstSheet="3" activeTab="4" xr2:uid="{28C085D8-E2A0-418F-8928-7A7EE2BAEA8D}"/>
   </bookViews>
   <sheets>
     <sheet name="prod_base_values" sheetId="1" r:id="rId1"/>
@@ -7994,8 +7994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B607FD-0A38-4A6B-A96A-ADA1BC478DD3}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8051,7 +8051,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="23">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -8068,7 +8068,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -8087,7 +8087,7 @@
         <v>150</v>
       </c>
       <c r="D6" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -8106,7 +8106,7 @@
         <v>2250</v>
       </c>
       <c r="D7" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -8144,7 +8144,7 @@
         <v>506250</v>
       </c>
       <c r="D9" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -8163,7 +8163,7 @@
         <v>7593750</v>
       </c>
       <c r="D10" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -8182,7 +8182,7 @@
         <v>113906250</v>
       </c>
       <c r="D11" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -8201,7 +8201,7 @@
         <v>1708593750</v>
       </c>
       <c r="D12" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -8220,7 +8220,7 @@
         <v>25628906250</v>
       </c>
       <c r="D13" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.06</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -8239,7 +8239,7 @@
         <v>384433593750</v>
       </c>
       <c r="D14" s="14">
-        <v>1.1000000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -8776,7 +8776,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9436,8 +9436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E531F0-085D-46CD-AA09-287683333E46}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9498,7 +9498,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" s="18">
         <v>0.1</v>

</xml_diff>

<commit_message>
Commit before changing to progressive PrestigeUpgrades method
</commit_message>
<xml_diff>
--- a/IdlePowerBalancing.xlsx
+++ b/IdlePowerBalancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\GitHub\IdlePowerBalancing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FC3FD7-DAD9-44A0-9DD0-16F3BC53B1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF5EEB7-5C11-43C6-BB55-B9DB58C1F9D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="743" firstSheet="2" activeTab="2" xr2:uid="{28C085D8-E2A0-418F-8928-7A7EE2BAEA8D}"/>
+    <workbookView xWindow="14303" yWindow="-4147" windowWidth="28995" windowHeight="15795" tabRatio="743" firstSheet="3" activeTab="10" xr2:uid="{28C085D8-E2A0-418F-8928-7A7EE2BAEA8D}"/>
   </bookViews>
   <sheets>
     <sheet name="prestige_values" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,6 @@
     <sheet name="demand_multi" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1476,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25FBFBAD-315E-452A-8A56-E96C8D5E9E73}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D40" sqref="D3:D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1525,7 @@
         <v>2000000</v>
       </c>
       <c r="D3" s="7">
-        <v>5.0000000000000002E+25</v>
+        <v>5000000000</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -1541,7 +1540,7 @@
       </c>
       <c r="D4" s="7">
         <f>D3*$C$3</f>
-        <v>1.0000000000000001E+32</v>
+        <v>1E+16</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -1556,7 +1555,7 @@
       </c>
       <c r="D5" s="7">
         <f t="shared" ref="D5:D40" si="0">D4*$C$3</f>
-        <v>2E+38</v>
+        <v>2E+22</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -1571,7 +1570,7 @@
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>3.9999999999999996E+44</v>
+        <v>3.9999999999999998E+28</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -1586,7 +1585,7 @@
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>7.9999999999999989E+50</v>
+        <v>7.9999999999999996E+34</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
@@ -1601,7 +1600,7 @@
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
-        <v>1.5999999999999998E+57</v>
+        <v>1.5999999999999999E+41</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -1616,7 +1615,7 @@
       </c>
       <c r="D9" s="7">
         <f t="shared" si="0"/>
-        <v>3.1999999999999997E+63</v>
+        <v>3.1999999999999996E+47</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
@@ -1631,7 +1630,7 @@
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>6.3999999999999997E+69</v>
+        <v>6.3999999999999991E+53</v>
       </c>
       <c r="E10" s="1">
         <v>4</v>
@@ -1646,7 +1645,7 @@
       </c>
       <c r="D11" s="7">
         <f t="shared" si="0"/>
-        <v>1.2799999999999999E+76</v>
+        <v>1.2799999999999997E+60</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
@@ -1662,7 +1661,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="7">
         <f t="shared" si="0"/>
-        <v>2.56E+82</v>
+        <v>2.5599999999999997E+66</v>
       </c>
       <c r="E12" s="12">
         <v>5</v>
@@ -1677,7 +1676,7 @@
       </c>
       <c r="D13" s="7">
         <f t="shared" si="0"/>
-        <v>5.1200000000000001E+88</v>
+        <v>5.1199999999999996E+72</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -1692,7 +1691,7 @@
       </c>
       <c r="D14" s="7">
         <f t="shared" si="0"/>
-        <v>1.024E+95</v>
+        <v>1.0239999999999999E+79</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1707,7 +1706,7 @@
       </c>
       <c r="D15" s="7">
         <f t="shared" si="0"/>
-        <v>2.048E+101</v>
+        <v>2.0479999999999999E+85</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -1722,7 +1721,7 @@
       </c>
       <c r="D16" s="7">
         <f t="shared" si="0"/>
-        <v>4.096E+107</v>
+        <v>4.0959999999999998E+91</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
@@ -1737,7 +1736,7 @@
       </c>
       <c r="D17" s="7">
         <f t="shared" si="0"/>
-        <v>8.1920000000000002E+113</v>
+        <v>8.1920000000000002E+97</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
@@ -1752,7 +1751,7 @@
       </c>
       <c r="D18" s="7">
         <f t="shared" si="0"/>
-        <v>1.6384E+120</v>
+        <v>1.6384E+104</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
@@ -1767,7 +1766,7 @@
       </c>
       <c r="D19" s="7">
         <f t="shared" si="0"/>
-        <v>3.2768E+126</v>
+        <v>3.2768000000000003E+110</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
@@ -1782,7 +1781,7 @@
       </c>
       <c r="D20" s="7">
         <f t="shared" si="0"/>
-        <v>6.5536000000000005E+132</v>
+        <v>6.5536000000000009E+116</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -1797,7 +1796,7 @@
       </c>
       <c r="D21" s="7">
         <f t="shared" si="0"/>
-        <v>1.3107200000000002E+139</v>
+        <v>1.3107200000000002E+123</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
@@ -1812,7 +1811,7 @@
       </c>
       <c r="D22" s="7">
         <f>D21*$C$3</f>
-        <v>2.6214400000000002E+145</v>
+        <v>2.6214400000000005E+129</v>
       </c>
       <c r="E22" s="1">
         <v>2</v>
@@ -1827,7 +1826,7 @@
       </c>
       <c r="D23" s="7">
         <f t="shared" si="0"/>
-        <v>5.2428800000000008E+151</v>
+        <v>5.242880000000001E+135</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
@@ -1842,7 +1841,7 @@
       </c>
       <c r="D24" s="7">
         <f t="shared" si="0"/>
-        <v>1.0485760000000002E+158</v>
+        <v>1.0485760000000002E+142</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
@@ -1857,7 +1856,7 @@
       </c>
       <c r="D25" s="7">
         <f t="shared" si="0"/>
-        <v>2.0971520000000004E+164</v>
+        <v>2.0971520000000004E+148</v>
       </c>
       <c r="E25" s="1">
         <v>2</v>
@@ -1869,7 +1868,7 @@
       </c>
       <c r="D26" s="7">
         <f>D25*$C$3</f>
-        <v>4.1943040000000011E+170</v>
+        <v>4.1943040000000008E+154</v>
       </c>
       <c r="E26" s="27">
         <v>2</v>
@@ -1881,7 +1880,7 @@
       </c>
       <c r="D27" s="7">
         <f t="shared" si="0"/>
-        <v>8.3886080000000025E+176</v>
+        <v>8.3886080000000016E+160</v>
       </c>
       <c r="E27" s="27">
         <v>2</v>
@@ -1893,7 +1892,7 @@
       </c>
       <c r="D28" s="7">
         <f t="shared" si="0"/>
-        <v>1.6777216000000005E+183</v>
+        <v>1.6777216000000003E+167</v>
       </c>
       <c r="E28" s="27">
         <v>2</v>
@@ -1905,7 +1904,7 @@
       </c>
       <c r="D29" s="7">
         <f t="shared" si="0"/>
-        <v>3.3554432000000012E+189</v>
+        <v>3.3554432000000003E+173</v>
       </c>
       <c r="E29" s="27">
         <v>2</v>
@@ -1917,7 +1916,7 @@
       </c>
       <c r="D30" s="7">
         <f t="shared" si="0"/>
-        <v>6.7108864000000022E+195</v>
+        <v>6.7108864000000006E+179</v>
       </c>
       <c r="E30" s="27">
         <v>2</v>
@@ -1929,7 +1928,7 @@
       </c>
       <c r="D31" s="7">
         <f t="shared" si="0"/>
-        <v>1.3421772800000004E+202</v>
+        <v>1.3421772800000001E+186</v>
       </c>
       <c r="E31" s="27">
         <v>2</v>
@@ -1943,7 +1942,7 @@
       <c r="C32" s="27"/>
       <c r="D32" s="7">
         <f>D31*$C$3</f>
-        <v>2.6843545600000008E+208</v>
+        <v>2.68435456E+192</v>
       </c>
       <c r="E32" s="27"/>
     </row>
@@ -1953,7 +1952,7 @@
       </c>
       <c r="D33" s="7">
         <f t="shared" si="0"/>
-        <v>5.3687091200000021E+214</v>
+        <v>5.3687091200000004E+198</v>
       </c>
       <c r="E33" s="27">
         <v>2</v>
@@ -1965,7 +1964,7 @@
       </c>
       <c r="D34" s="7">
         <f t="shared" si="0"/>
-        <v>1.0737418240000005E+221</v>
+        <v>1.0737418240000002E+205</v>
       </c>
       <c r="E34" s="27">
         <v>2</v>
@@ -1977,7 +1976,7 @@
       </c>
       <c r="D35" s="7">
         <f t="shared" si="0"/>
-        <v>2.147483648000001E+227</v>
+        <v>2.1474836480000003E+211</v>
       </c>
       <c r="E35" s="27">
         <v>2</v>
@@ -1989,7 +1988,7 @@
       </c>
       <c r="D36" s="7">
         <f t="shared" si="0"/>
-        <v>4.2949672960000016E+233</v>
+        <v>4.2949672960000004E+217</v>
       </c>
       <c r="E36" s="27">
         <v>2</v>
@@ -2001,7 +2000,7 @@
       </c>
       <c r="D37" s="7">
         <f t="shared" si="0"/>
-        <v>8.5899345920000027E+239</v>
+        <v>8.5899345920000006E+223</v>
       </c>
       <c r="E37" s="27">
         <v>2</v>
@@ -2013,7 +2012,7 @@
       </c>
       <c r="D38" s="7">
         <f t="shared" si="0"/>
-        <v>1.7179869184000005E+246</v>
+        <v>1.7179869184000002E+230</v>
       </c>
       <c r="E38" s="27">
         <v>2</v>
@@ -2025,7 +2024,7 @@
       </c>
       <c r="D39" s="7">
         <f t="shared" si="0"/>
-        <v>3.435973836800001E+252</v>
+        <v>3.4359738368000003E+236</v>
       </c>
       <c r="E39" s="27">
         <v>2</v>
@@ -2037,7 +2036,7 @@
       </c>
       <c r="D40" s="7">
         <f t="shared" si="0"/>
-        <v>6.871947673600002E+258</v>
+        <v>6.8719476736000004E+242</v>
       </c>
       <c r="E40" s="27">
         <v>2</v>
@@ -2348,7 +2347,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="20">
-        <v>5.0000000000000002E+25</v>
+        <v>9000000000</v>
       </c>
       <c r="D4" s="13">
         <v>2</v>
@@ -2413,7 +2412,7 @@
       </c>
       <c r="C5" s="20">
         <f>C4*C$3</f>
-        <v>1.0000000000000001E+32</v>
+        <v>1.8E+16</v>
       </c>
       <c r="D5" s="13">
         <v>2</v>
@@ -2428,7 +2427,7 @@
       </c>
       <c r="C6" s="20">
         <f t="shared" ref="C6:C33" si="0">C5*C$3</f>
-        <v>2E+38</v>
+        <v>3.6E+22</v>
       </c>
       <c r="D6" s="13">
         <v>2</v>
@@ -2443,7 +2442,7 @@
       </c>
       <c r="C7" s="20">
         <f t="shared" si="0"/>
-        <v>3.9999999999999996E+44</v>
+        <v>7.1999999999999999E+28</v>
       </c>
       <c r="D7" s="13">
         <v>2</v>
@@ -2458,7 +2457,7 @@
       </c>
       <c r="C8" s="20">
         <f t="shared" si="0"/>
-        <v>7.9999999999999989E+50</v>
+        <v>1.44E+35</v>
       </c>
       <c r="D8" s="13">
         <v>2</v>
@@ -2473,7 +2472,7 @@
       </c>
       <c r="C9" s="20">
         <f t="shared" si="0"/>
-        <v>1.5999999999999998E+57</v>
+        <v>2.88E+41</v>
       </c>
       <c r="D9" s="13">
         <v>2</v>
@@ -2488,7 +2487,7 @@
       </c>
       <c r="C10" s="20">
         <f t="shared" si="0"/>
-        <v>3.1999999999999997E+63</v>
+        <v>5.7599999999999998E+47</v>
       </c>
       <c r="D10" s="13">
         <v>2</v>
@@ -2503,7 +2502,7 @@
       </c>
       <c r="C11" s="20">
         <f t="shared" si="0"/>
-        <v>6.3999999999999997E+69</v>
+        <v>1.152E+54</v>
       </c>
       <c r="D11" s="13">
         <v>2</v>
@@ -2518,7 +2517,7 @@
       </c>
       <c r="C12" s="20">
         <f t="shared" si="0"/>
-        <v>1.2799999999999999E+76</v>
+        <v>2.304E+60</v>
       </c>
       <c r="D12" s="13">
         <v>2</v>
@@ -2533,7 +2532,7 @@
       </c>
       <c r="C13" s="20">
         <f t="shared" si="0"/>
-        <v>2.56E+82</v>
+        <v>4.6080000000000002E+66</v>
       </c>
       <c r="D13" s="13">
         <v>2</v>
@@ -2548,7 +2547,7 @@
       </c>
       <c r="C14" s="20">
         <f t="shared" si="0"/>
-        <v>5.1200000000000001E+88</v>
+        <v>9.2159999999999999E+72</v>
       </c>
       <c r="D14" s="13">
         <v>2</v>
@@ -2563,7 +2562,7 @@
       </c>
       <c r="C15" s="20">
         <f t="shared" si="0"/>
-        <v>1.024E+95</v>
+        <v>1.8431999999999998E+79</v>
       </c>
       <c r="D15" s="13">
         <v>2</v>
@@ -2578,7 +2577,7 @@
       </c>
       <c r="C16" s="20">
         <f t="shared" si="0"/>
-        <v>2.048E+101</v>
+        <v>3.6863999999999995E+85</v>
       </c>
       <c r="D16" s="13">
         <v>2</v>
@@ -2593,7 +2592,7 @@
       </c>
       <c r="C17" s="20">
         <f t="shared" si="0"/>
-        <v>4.096E+107</v>
+        <v>7.372799999999999E+91</v>
       </c>
       <c r="D17" s="13">
         <v>2</v>
@@ -2608,7 +2607,7 @@
       </c>
       <c r="C18" s="20">
         <f t="shared" si="0"/>
-        <v>8.1920000000000002E+113</v>
+        <v>1.4745599999999997E+98</v>
       </c>
       <c r="D18" s="13">
         <v>2</v>
@@ -2623,7 +2622,7 @@
       </c>
       <c r="C19" s="20">
         <f t="shared" si="0"/>
-        <v>1.6384E+120</v>
+        <v>2.9491199999999993E+104</v>
       </c>
       <c r="D19" s="13">
         <v>2</v>
@@ -2638,7 +2637,7 @@
       </c>
       <c r="C20" s="20">
         <f t="shared" si="0"/>
-        <v>3.2768E+126</v>
+        <v>5.8982399999999988E+110</v>
       </c>
       <c r="D20" s="13">
         <v>2</v>
@@ -2653,7 +2652,7 @@
       </c>
       <c r="C21" s="20">
         <f t="shared" si="0"/>
-        <v>6.5536000000000005E+132</v>
+        <v>1.1796479999999997E+117</v>
       </c>
       <c r="D21" s="13">
         <v>2</v>
@@ -2668,7 +2667,7 @@
       </c>
       <c r="C22" s="20">
         <f t="shared" si="0"/>
-        <v>1.3107200000000002E+139</v>
+        <v>2.3592959999999994E+123</v>
       </c>
       <c r="D22" s="13">
         <v>2</v>
@@ -2683,7 +2682,7 @@
       </c>
       <c r="C23" s="20">
         <f t="shared" si="0"/>
-        <v>2.6214400000000002E+145</v>
+        <v>4.7185919999999986E+129</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -2698,7 +2697,7 @@
       </c>
       <c r="C24" s="20">
         <f>C23*C$3</f>
-        <v>5.2428800000000008E+151</v>
+        <v>9.4371839999999977E+135</v>
       </c>
       <c r="D24" s="13">
         <v>2</v>
@@ -2713,7 +2712,7 @@
       </c>
       <c r="C25" s="20">
         <f t="shared" si="0"/>
-        <v>1.0485760000000002E+158</v>
+        <v>1.8874367999999995E+142</v>
       </c>
       <c r="D25" s="13">
         <v>2</v>
@@ -2728,7 +2727,7 @@
       </c>
       <c r="C26" s="20">
         <f t="shared" si="0"/>
-        <v>2.0971520000000004E+164</v>
+        <v>3.774873599999999E+148</v>
       </c>
       <c r="D26" s="13">
         <v>2</v>
@@ -2740,7 +2739,7 @@
       </c>
       <c r="C27" s="20">
         <f t="shared" si="0"/>
-        <v>4.1943040000000011E+170</v>
+        <v>7.5497471999999977E+154</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
@@ -2752,7 +2751,7 @@
       </c>
       <c r="C28" s="20">
         <f t="shared" si="0"/>
-        <v>8.3886080000000025E+176</v>
+        <v>1.5099494399999995E+161</v>
       </c>
       <c r="D28" s="13">
         <v>2</v>
@@ -2764,7 +2763,7 @@
       </c>
       <c r="C29" s="20">
         <f t="shared" si="0"/>
-        <v>1.6777216000000005E+183</v>
+        <v>3.0198988799999991E+167</v>
       </c>
       <c r="D29" s="13">
         <v>2</v>
@@ -2777,7 +2776,7 @@
       <c r="B30" s="27"/>
       <c r="C30" s="20">
         <f>C29*C$3</f>
-        <v>3.3554432000000012E+189</v>
+        <v>6.0397977599999984E+173</v>
       </c>
       <c r="D30" s="13">
         <v>2</v>
@@ -2790,7 +2789,7 @@
       <c r="B31" s="27"/>
       <c r="C31" s="20">
         <f t="shared" si="0"/>
-        <v>6.7108864000000022E+195</v>
+        <v>1.2079595519999997E+180</v>
       </c>
       <c r="D31" s="13">
         <v>2</v>
@@ -2802,7 +2801,7 @@
       </c>
       <c r="C32" s="20">
         <f t="shared" si="0"/>
-        <v>1.3421772800000004E+202</v>
+        <v>2.4159191039999994E+186</v>
       </c>
       <c r="D32" s="13">
         <v>2</v>
@@ -2814,7 +2813,7 @@
       </c>
       <c r="C33" s="20">
         <f t="shared" si="0"/>
-        <v>2.6843545600000008E+208</v>
+        <v>4.8318382079999992E+192</v>
       </c>
       <c r="D33" s="13">
         <v>2</v>
@@ -2827,7 +2826,7 @@
       <c r="B34" s="27"/>
       <c r="C34" s="20">
         <f>C33*C$3</f>
-        <v>5.3687091200000021E+214</v>
+        <v>9.6636764159999973E+198</v>
       </c>
       <c r="D34" s="13">
         <v>2</v>
@@ -2839,7 +2838,7 @@
       </c>
       <c r="C35" s="20">
         <f>C34*C$3</f>
-        <v>1.0737418240000005E+221</v>
+        <v>1.9327352831999994E+205</v>
       </c>
       <c r="D35" s="13">
         <v>2</v>
@@ -2852,7 +2851,7 @@
       <c r="B36" s="27"/>
       <c r="C36" s="20">
         <f>C35*C$3</f>
-        <v>2.147483648000001E+227</v>
+        <v>3.8654705663999987E+211</v>
       </c>
       <c r="D36" s="13">
         <v>2</v>
@@ -2864,7 +2863,7 @@
       </c>
       <c r="C37" s="20">
         <f t="shared" ref="C37:C41" si="1">C36*C$3</f>
-        <v>4.2949672960000016E+233</v>
+        <v>7.7309411327999971E+217</v>
       </c>
       <c r="D37" s="13">
         <v>2</v>
@@ -2877,7 +2876,7 @@
       <c r="B38" s="27"/>
       <c r="C38" s="20">
         <f t="shared" si="1"/>
-        <v>8.5899345920000027E+239</v>
+        <v>1.5461882265599994E+224</v>
       </c>
       <c r="D38" s="13">
         <v>2</v>
@@ -2890,7 +2889,7 @@
       <c r="B39" s="27"/>
       <c r="C39" s="20">
         <f t="shared" si="1"/>
-        <v>1.7179869184000005E+246</v>
+        <v>3.0923764531199989E+230</v>
       </c>
       <c r="D39" s="13">
         <v>2</v>
@@ -2902,7 +2901,7 @@
       </c>
       <c r="C40" s="20">
         <f t="shared" si="1"/>
-        <v>3.435973836800001E+252</v>
+        <v>6.1847529062399979E+236</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2911,7 +2910,7 @@
       </c>
       <c r="C41" s="20">
         <f t="shared" si="1"/>
-        <v>6.871947673600002E+258</v>
+        <v>1.2369505812479996E+243</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3610,7 +3609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B607FD-0A38-4A6B-A96A-ADA1BC478DD3}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>